<commit_message>
change the properties of obj
</commit_message>
<xml_diff>
--- a/TaskDistribution.xlsx
+++ b/TaskDistribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\cybersoft\32E_NgocvsDang_ShoesShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905596FD-75C4-4BB6-AB6C-37AA6C2FEC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63530C9-0E67-425C-B7E5-C33E085FEBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,13 +75,7 @@
     <t>Ngọc</t>
   </si>
   <si>
-    <t>index.html</t>
-  </si>
-  <si>
     <t>footer</t>
-  </si>
-  <si>
-    <t>detail.html</t>
   </si>
   <si>
     <t>Main content</t>
@@ -90,13 +84,19 @@
     <t>Feature-product</t>
   </si>
   <si>
-    <t>register.html</t>
-  </si>
-  <si>
     <t>Menu</t>
   </si>
   <si>
     <t>form</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>register</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -314,19 +314,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -492,19 +479,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="9" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -657,19 +631,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color theme="9" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -761,32 +722,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -805,41 +744,41 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,24 +794,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -884,111 +807,111 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1220,10 +1143,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O983"/>
+  <dimension ref="A1:O979"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1240,196 +1163,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="66" t="s">
+      <c r="K1" s="50" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="21">
         <v>44628</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="21">
         <v>44659</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="22">
         <v>1</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="77" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="78"/>
-      <c r="N2" s="79"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="29">
+      <c r="A3" s="55"/>
+      <c r="B3" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="21">
         <v>44628</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="21">
         <v>44659</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="82"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="65"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="21">
         <v>44628</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="21">
         <v>44659</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="85"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="68"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="29">
+        <v>16</v>
+      </c>
+      <c r="C5" s="21">
         <v>44689</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="21">
         <v>44689</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="22">
         <v>1</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="85"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="68"/>
     </row>
     <row r="6" spans="1:15" ht="19.8" customHeight="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
-      <c r="B6" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="29">
+      <c r="A6" s="56"/>
+      <c r="B6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="21">
         <v>44689</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="21">
         <v>44689</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="88"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="71"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="89" t="s">
+      <c r="A7" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="90"/>
-      <c r="N7" s="91"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="10"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1439,14 +1362,14 @@
       <c r="H8" s="8"/>
       <c r="I8" s="9"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="57"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="42"/>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="10"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1456,14 +1379,14 @@
       <c r="H9" s="8"/>
       <c r="I9" s="9"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="57"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="42"/>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="10"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1473,123 +1396,62 @@
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="85"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="68"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="88"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="71"/>
     </row>
     <row r="12" spans="1:15" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="40" t="s">
+      <c r="A12" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="41">
+      <c r="B12" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="33">
         <v>44720</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="33">
         <v>44750</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="89" t="s">
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="90"/>
-      <c r="N12" s="91"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="77"/>
     </row>
-    <row r="13" spans="1:15" ht="19.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="57"/>
-    </row>
-    <row r="14" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="85"/>
-    </row>
-    <row r="15" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="85"/>
-    </row>
-    <row r="16" spans="1:15" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="76"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="88"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2552,20 +2414,14 @@
     <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
     <mergeCell ref="L2:N6"/>
     <mergeCell ref="L7:N11"/>
-    <mergeCell ref="L12:N16"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E11 I4:I16 E13:E16">
+  <conditionalFormatting sqref="E7:E11 I4:I12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>